<commit_message>
Refine ga code for review
</commit_message>
<xml_diff>
--- a/GA/src/result.xlsx
+++ b/GA/src/result.xlsx
@@ -478,7 +478,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>195248</v>
+        <v>328018</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -497,7 +497,7 @@
         <v>5</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -519,7 +519,7 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -530,7 +530,7 @@
         <v>6</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -544,7 +544,7 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -555,7 +555,7 @@
         <v>6</v>
       </c>
       <c r="D10">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -566,7 +566,7 @@
         <v>5</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -577,7 +577,7 @@
         <v>6</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -596,7 +596,7 @@
         <v>5</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -607,7 +607,7 @@
         <v>6</v>
       </c>
       <c r="D16">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -618,7 +618,7 @@
         <v>5</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -629,7 +629,7 @@
         <v>6</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -643,7 +643,7 @@
         <v>5</v>
       </c>
       <c r="D19">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -654,7 +654,7 @@
         <v>6</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -665,7 +665,7 @@
         <v>5</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -676,7 +676,7 @@
         <v>6</v>
       </c>
       <c r="D22">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -698,7 +698,7 @@
         <v>5</v>
       </c>
       <c r="E25">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -709,7 +709,7 @@
         <v>6</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -720,7 +720,7 @@
         <v>5</v>
       </c>
       <c r="E27">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -731,7 +731,7 @@
         <v>6</v>
       </c>
       <c r="E28">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -745,7 +745,7 @@
         <v>5</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -767,7 +767,7 @@
         <v>5</v>
       </c>
       <c r="E31">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -778,7 +778,7 @@
         <v>6</v>
       </c>
       <c r="E32">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -806,7 +806,7 @@
         <v>6</v>
       </c>
       <c r="E34">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -817,7 +817,7 @@
         <v>5</v>
       </c>
       <c r="E35">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -828,7 +828,7 @@
         <v>6</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -853,7 +853,7 @@
         <v>6</v>
       </c>
       <c r="E38">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -900,7 +900,7 @@
         <v>5</v>
       </c>
       <c r="F43">
-        <v>100</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -911,7 +911,7 @@
         <v>6</v>
       </c>
       <c r="F44">
-        <v>27</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -922,7 +922,7 @@
         <v>5</v>
       </c>
       <c r="F45">
-        <v>132</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -933,7 +933,7 @@
         <v>6</v>
       </c>
       <c r="F46">
-        <v>43</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -947,7 +947,7 @@
         <v>5</v>
       </c>
       <c r="F47">
-        <v>156</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -958,7 +958,7 @@
         <v>6</v>
       </c>
       <c r="F48">
-        <v>22</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -969,7 +969,7 @@
         <v>5</v>
       </c>
       <c r="F49">
-        <v>26</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -980,7 +980,7 @@
         <v>6</v>
       </c>
       <c r="F50">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -997,7 +997,7 @@
         <v>5</v>
       </c>
       <c r="F51">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1008,7 +1008,7 @@
         <v>6</v>
       </c>
       <c r="F52">
-        <v>68</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1019,7 +1019,7 @@
         <v>5</v>
       </c>
       <c r="F53">
-        <v>134</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1030,7 +1030,7 @@
         <v>6</v>
       </c>
       <c r="F54">
-        <v>82</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1044,7 +1044,7 @@
         <v>5</v>
       </c>
       <c r="F55">
-        <v>132</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1055,7 +1055,7 @@
         <v>6</v>
       </c>
       <c r="F56">
-        <v>23</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1066,7 +1066,7 @@
         <v>5</v>
       </c>
       <c r="F57">
-        <v>24</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1077,7 +1077,7 @@
         <v>6</v>
       </c>
       <c r="F58">
-        <v>59</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1097,7 +1097,7 @@
         <v>5</v>
       </c>
       <c r="F59">
-        <v>80</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1108,7 +1108,7 @@
         <v>6</v>
       </c>
       <c r="F60">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1119,7 +1119,7 @@
         <v>5</v>
       </c>
       <c r="F61">
-        <v>22</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1130,7 +1130,7 @@
         <v>6</v>
       </c>
       <c r="F62">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1144,7 +1144,7 @@
         <v>5</v>
       </c>
       <c r="F63">
-        <v>8</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1155,7 +1155,7 @@
         <v>6</v>
       </c>
       <c r="F64">
-        <v>128</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1166,7 +1166,7 @@
         <v>5</v>
       </c>
       <c r="F65">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1177,7 +1177,7 @@
         <v>6</v>
       </c>
       <c r="F66">
-        <v>43</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1194,7 +1194,7 @@
         <v>5</v>
       </c>
       <c r="F67">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1205,7 +1205,7 @@
         <v>6</v>
       </c>
       <c r="F68">
-        <v>106</v>
+        <v>37</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1216,7 +1216,7 @@
         <v>5</v>
       </c>
       <c r="F69">
-        <v>77</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1227,7 +1227,7 @@
         <v>6</v>
       </c>
       <c r="F70">
-        <v>13</v>
+        <v>47</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1241,7 +1241,7 @@
         <v>5</v>
       </c>
       <c r="F71">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1252,7 +1252,7 @@
         <v>6</v>
       </c>
       <c r="F72">
-        <v>94</v>
+        <v>151</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -1263,7 +1263,7 @@
         <v>5</v>
       </c>
       <c r="F73">
-        <v>78</v>
+        <v>95</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -1274,7 +1274,7 @@
         <v>6</v>
       </c>
       <c r="F74">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -1293,7 +1293,7 @@
         <v>5</v>
       </c>
       <c r="D77">
-        <v>65</v>
+        <v>37</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -1304,7 +1304,7 @@
         <v>6</v>
       </c>
       <c r="D78">
-        <v>70</v>
+        <v>38</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -1315,7 +1315,7 @@
         <v>5</v>
       </c>
       <c r="D79">
-        <v>63</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -1326,7 +1326,7 @@
         <v>6</v>
       </c>
       <c r="D80">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1340,7 +1340,7 @@
         <v>5</v>
       </c>
       <c r="D81">
-        <v>86</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1351,7 +1351,7 @@
         <v>6</v>
       </c>
       <c r="D82">
-        <v>89</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1362,7 +1362,7 @@
         <v>5</v>
       </c>
       <c r="D83">
-        <v>52</v>
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1373,7 +1373,7 @@
         <v>6</v>
       </c>
       <c r="D84">
-        <v>4</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1389,7 +1389,7 @@
         <v>5</v>
       </c>
       <c r="C87">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1397,7 +1397,7 @@
         <v>6</v>
       </c>
       <c r="C88">
-        <v>8</v>
+        <v>419</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1408,7 +1408,7 @@
         <v>5</v>
       </c>
       <c r="C89">
-        <v>1109</v>
+        <v>159</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1416,7 +1416,7 @@
         <v>6</v>
       </c>
       <c r="C90">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1432,7 +1432,7 @@
         <v>5</v>
       </c>
       <c r="C93">
-        <v>27</v>
+        <v>576</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1440,7 +1440,7 @@
         <v>6</v>
       </c>
       <c r="C94">
-        <v>2512</v>
+        <v>392</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1451,7 +1451,7 @@
         <v>5</v>
       </c>
       <c r="C95">
-        <v>110</v>
+        <v>811</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1459,7 +1459,7 @@
         <v>6</v>
       </c>
       <c r="C96">
-        <v>489</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -1478,7 +1478,7 @@
         <v>5</v>
       </c>
       <c r="D99">
-        <v>488</v>
+        <v>728</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1489,7 +1489,7 @@
         <v>6</v>
       </c>
       <c r="D100">
-        <v>87</v>
+        <v>721</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1500,7 +1500,7 @@
         <v>5</v>
       </c>
       <c r="D101">
-        <v>330</v>
+        <v>246</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1511,7 +1511,7 @@
         <v>6</v>
       </c>
       <c r="D102">
-        <v>844</v>
+        <v>469</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -1525,7 +1525,7 @@
         <v>5</v>
       </c>
       <c r="D103">
-        <v>726</v>
+        <v>122</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1536,7 +1536,7 @@
         <v>6</v>
       </c>
       <c r="D104">
-        <v>205</v>
+        <v>354</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -1547,7 +1547,7 @@
         <v>5</v>
       </c>
       <c r="D105">
-        <v>589</v>
+        <v>603</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -1558,7 +1558,7 @@
         <v>6</v>
       </c>
       <c r="D106">
-        <v>2</v>
+        <v>267</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -1577,7 +1577,7 @@
         <v>5</v>
       </c>
       <c r="D109">
-        <v>234</v>
+        <v>64</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -1588,7 +1588,7 @@
         <v>6</v>
       </c>
       <c r="D110">
-        <v>289</v>
+        <v>452</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -1599,7 +1599,7 @@
         <v>5</v>
       </c>
       <c r="D111">
-        <v>5</v>
+        <v>346</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -1610,7 +1610,7 @@
         <v>6</v>
       </c>
       <c r="D112">
-        <v>1</v>
+        <v>201</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -1624,7 +1624,7 @@
         <v>5</v>
       </c>
       <c r="D113">
-        <v>217</v>
+        <v>124</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -1635,7 +1635,7 @@
         <v>6</v>
       </c>
       <c r="D114">
-        <v>62</v>
+        <v>433</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -1646,7 +1646,7 @@
         <v>5</v>
       </c>
       <c r="D115">
-        <v>383</v>
+        <v>361</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -1657,7 +1657,7 @@
         <v>6</v>
       </c>
       <c r="D116">
-        <v>13</v>
+        <v>256</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -1679,7 +1679,7 @@
         <v>5</v>
       </c>
       <c r="E119">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -1690,7 +1690,7 @@
         <v>6</v>
       </c>
       <c r="E120">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -1701,7 +1701,7 @@
         <v>5</v>
       </c>
       <c r="E121">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -1712,7 +1712,7 @@
         <v>6</v>
       </c>
       <c r="E122">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -1726,7 +1726,7 @@
         <v>5</v>
       </c>
       <c r="E123">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -1737,7 +1737,7 @@
         <v>6</v>
       </c>
       <c r="E124">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -1748,7 +1748,7 @@
         <v>5</v>
       </c>
       <c r="E125">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -1759,7 +1759,7 @@
         <v>6</v>
       </c>
       <c r="E126">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -1776,7 +1776,7 @@
         <v>5</v>
       </c>
       <c r="E127">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -1787,7 +1787,7 @@
         <v>6</v>
       </c>
       <c r="E128">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -1798,7 +1798,7 @@
         <v>5</v>
       </c>
       <c r="E129">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -1823,7 +1823,7 @@
         <v>5</v>
       </c>
       <c r="E131">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -1834,7 +1834,7 @@
         <v>6</v>
       </c>
       <c r="E132">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -1845,7 +1845,7 @@
         <v>5</v>
       </c>
       <c r="E133">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -1856,7 +1856,7 @@
         <v>6</v>
       </c>
       <c r="E134">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -1875,7 +1875,7 @@
         <v>5</v>
       </c>
       <c r="D137">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -1886,7 +1886,7 @@
         <v>6</v>
       </c>
       <c r="D138">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -1897,7 +1897,7 @@
         <v>5</v>
       </c>
       <c r="D139">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -1908,7 +1908,7 @@
         <v>6</v>
       </c>
       <c r="D140">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -1922,7 +1922,7 @@
         <v>5</v>
       </c>
       <c r="D141">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -1933,7 +1933,7 @@
         <v>6</v>
       </c>
       <c r="D142">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -1944,7 +1944,7 @@
         <v>5</v>
       </c>
       <c r="D143">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -1955,7 +1955,7 @@
         <v>6</v>
       </c>
       <c r="D144">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -1974,7 +1974,7 @@
         <v>5</v>
       </c>
       <c r="D147">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -1996,7 +1996,7 @@
         <v>5</v>
       </c>
       <c r="D149">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -2043,7 +2043,7 @@
         <v>5</v>
       </c>
       <c r="D153">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -2073,7 +2073,7 @@
         <v>5</v>
       </c>
       <c r="D157">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -2095,7 +2095,7 @@
         <v>5</v>
       </c>
       <c r="D159">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -2142,7 +2142,7 @@
         <v>5</v>
       </c>
       <c r="D163">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -2175,7 +2175,7 @@
         <v>5</v>
       </c>
       <c r="E167">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -2186,7 +2186,7 @@
         <v>6</v>
       </c>
       <c r="E168">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -2197,7 +2197,7 @@
         <v>5</v>
       </c>
       <c r="E169">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -2208,7 +2208,7 @@
         <v>6</v>
       </c>
       <c r="E170">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -2233,7 +2233,7 @@
         <v>6</v>
       </c>
       <c r="E172">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -2244,7 +2244,7 @@
         <v>5</v>
       </c>
       <c r="E173">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -2255,7 +2255,7 @@
         <v>6</v>
       </c>
       <c r="E174">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -2272,7 +2272,7 @@
         <v>5</v>
       </c>
       <c r="E175">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -2283,7 +2283,7 @@
         <v>6</v>
       </c>
       <c r="E176">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:6">
@@ -2305,7 +2305,7 @@
         <v>6</v>
       </c>
       <c r="E178">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179" spans="1:6">
@@ -2319,7 +2319,7 @@
         <v>5</v>
       </c>
       <c r="E179">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:6">
@@ -2330,7 +2330,7 @@
         <v>6</v>
       </c>
       <c r="E180">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181" spans="1:6">
@@ -2377,7 +2377,7 @@
         <v>5</v>
       </c>
       <c r="F185">
-        <v>65</v>
+        <v>29</v>
       </c>
     </row>
     <row r="186" spans="1:6">
@@ -2388,7 +2388,7 @@
         <v>6</v>
       </c>
       <c r="F186">
-        <v>35</v>
+        <v>95</v>
       </c>
     </row>
     <row r="187" spans="1:6">
@@ -2399,7 +2399,7 @@
         <v>5</v>
       </c>
       <c r="F187">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="188" spans="1:6">
@@ -2410,7 +2410,7 @@
         <v>6</v>
       </c>
       <c r="F188">
-        <v>6</v>
+        <v>86</v>
       </c>
     </row>
     <row r="189" spans="1:6">
@@ -2424,7 +2424,7 @@
         <v>5</v>
       </c>
       <c r="F189">
-        <v>73</v>
+        <v>38</v>
       </c>
     </row>
     <row r="190" spans="1:6">
@@ -2435,7 +2435,7 @@
         <v>6</v>
       </c>
       <c r="F190">
-        <v>97</v>
+        <v>57</v>
       </c>
     </row>
     <row r="191" spans="1:6">
@@ -2446,7 +2446,7 @@
         <v>5</v>
       </c>
       <c r="F191">
-        <v>6</v>
+        <v>34</v>
       </c>
     </row>
     <row r="192" spans="1:6">
@@ -2457,7 +2457,7 @@
         <v>6</v>
       </c>
       <c r="F192">
-        <v>29</v>
+        <v>74</v>
       </c>
     </row>
     <row r="193" spans="1:6">
@@ -2474,7 +2474,7 @@
         <v>5</v>
       </c>
       <c r="F193">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="194" spans="1:6">
@@ -2485,7 +2485,7 @@
         <v>6</v>
       </c>
       <c r="F194">
-        <v>69</v>
+        <v>3</v>
       </c>
     </row>
     <row r="195" spans="1:6">
@@ -2496,7 +2496,7 @@
         <v>5</v>
       </c>
       <c r="F195">
-        <v>23</v>
+        <v>67</v>
       </c>
     </row>
     <row r="196" spans="1:6">
@@ -2507,7 +2507,7 @@
         <v>6</v>
       </c>
       <c r="F196">
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
     <row r="197" spans="1:6">
@@ -2521,7 +2521,7 @@
         <v>5</v>
       </c>
       <c r="F197">
-        <v>82</v>
+        <v>21</v>
       </c>
     </row>
     <row r="198" spans="1:6">
@@ -2532,7 +2532,7 @@
         <v>6</v>
       </c>
       <c r="F198">
-        <v>50</v>
+        <v>23</v>
       </c>
     </row>
     <row r="199" spans="1:6">
@@ -2543,7 +2543,7 @@
         <v>5</v>
       </c>
       <c r="F199">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="200" spans="1:6">
@@ -2554,7 +2554,7 @@
         <v>6</v>
       </c>
       <c r="F200">
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="201" spans="1:6">
@@ -2574,7 +2574,7 @@
         <v>5</v>
       </c>
       <c r="F201">
-        <v>59</v>
+        <v>78</v>
       </c>
     </row>
     <row r="202" spans="1:6">
@@ -2585,7 +2585,7 @@
         <v>6</v>
       </c>
       <c r="F202">
-        <v>12</v>
+        <v>94</v>
       </c>
     </row>
     <row r="203" spans="1:6">
@@ -2596,7 +2596,7 @@
         <v>5</v>
       </c>
       <c r="F203">
-        <v>85</v>
+        <v>45</v>
       </c>
     </row>
     <row r="204" spans="1:6">
@@ -2607,7 +2607,7 @@
         <v>6</v>
       </c>
       <c r="F204">
-        <v>68</v>
+        <v>9</v>
       </c>
     </row>
     <row r="205" spans="1:6">
@@ -2621,7 +2621,7 @@
         <v>5</v>
       </c>
       <c r="F205">
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row r="206" spans="1:6">
@@ -2632,7 +2632,7 @@
         <v>6</v>
       </c>
       <c r="F206">
-        <v>3</v>
+        <v>82</v>
       </c>
     </row>
     <row r="207" spans="1:6">
@@ -2643,7 +2643,7 @@
         <v>5</v>
       </c>
       <c r="F207">
-        <v>37</v>
+        <v>71</v>
       </c>
     </row>
     <row r="208" spans="1:6">
@@ -2654,7 +2654,7 @@
         <v>6</v>
       </c>
       <c r="F208">
-        <v>94</v>
+        <v>36</v>
       </c>
     </row>
     <row r="209" spans="1:6">
@@ -2671,7 +2671,7 @@
         <v>5</v>
       </c>
       <c r="F209">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="210" spans="1:6">
@@ -2682,7 +2682,7 @@
         <v>6</v>
       </c>
       <c r="F210">
-        <v>3</v>
+        <v>92</v>
       </c>
     </row>
     <row r="211" spans="1:6">
@@ -2693,7 +2693,7 @@
         <v>5</v>
       </c>
       <c r="F211">
-        <v>53</v>
+        <v>13</v>
       </c>
     </row>
     <row r="212" spans="1:6">
@@ -2704,7 +2704,7 @@
         <v>6</v>
       </c>
       <c r="F212">
-        <v>27</v>
+        <v>63</v>
       </c>
     </row>
     <row r="213" spans="1:6">
@@ -2718,7 +2718,7 @@
         <v>5</v>
       </c>
       <c r="F213">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="214" spans="1:6">
@@ -2729,7 +2729,7 @@
         <v>6</v>
       </c>
       <c r="F214">
-        <v>63</v>
+        <v>2</v>
       </c>
     </row>
     <row r="215" spans="1:6">
@@ -2740,7 +2740,7 @@
         <v>5</v>
       </c>
       <c r="F215">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="216" spans="1:6">
@@ -2751,7 +2751,7 @@
         <v>6</v>
       </c>
       <c r="F216">
-        <v>89</v>
+        <v>27</v>
       </c>
     </row>
     <row r="218" spans="1:6">
@@ -2773,7 +2773,7 @@
         <v>5</v>
       </c>
       <c r="E219">
-        <v>12</v>
+        <v>103</v>
       </c>
     </row>
     <row r="220" spans="1:6">
@@ -2784,7 +2784,7 @@
         <v>6</v>
       </c>
       <c r="E220">
-        <v>108</v>
+        <v>3</v>
       </c>
     </row>
     <row r="221" spans="1:6">
@@ -2795,7 +2795,7 @@
         <v>5</v>
       </c>
       <c r="E221">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="222" spans="1:6">
@@ -2806,7 +2806,7 @@
         <v>6</v>
       </c>
       <c r="E222">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="223" spans="1:6">
@@ -2820,7 +2820,7 @@
         <v>5</v>
       </c>
       <c r="E223">
-        <v>113</v>
+        <v>129</v>
       </c>
     </row>
     <row r="224" spans="1:6">
@@ -2831,7 +2831,7 @@
         <v>6</v>
       </c>
       <c r="E224">
-        <v>116</v>
+        <v>95</v>
       </c>
     </row>
     <row r="225" spans="1:5">
@@ -2842,7 +2842,7 @@
         <v>5</v>
       </c>
       <c r="E225">
-        <v>16</v>
+        <v>130</v>
       </c>
     </row>
     <row r="226" spans="1:5">
@@ -2853,7 +2853,7 @@
         <v>6</v>
       </c>
       <c r="E226">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="227" spans="1:5">
@@ -2870,7 +2870,7 @@
         <v>5</v>
       </c>
       <c r="E227">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="228" spans="1:5">
@@ -2881,7 +2881,7 @@
         <v>6</v>
       </c>
       <c r="E228">
-        <v>25</v>
+        <v>52</v>
       </c>
     </row>
     <row r="229" spans="1:5">
@@ -2892,7 +2892,7 @@
         <v>5</v>
       </c>
       <c r="E229">
-        <v>37</v>
+        <v>6</v>
       </c>
     </row>
     <row r="230" spans="1:5">
@@ -2903,7 +2903,7 @@
         <v>6</v>
       </c>
       <c r="E230">
-        <v>58</v>
+        <v>132</v>
       </c>
     </row>
     <row r="231" spans="1:5">
@@ -2917,7 +2917,7 @@
         <v>5</v>
       </c>
       <c r="E231">
-        <v>3</v>
+        <v>119</v>
       </c>
     </row>
     <row r="232" spans="1:5">
@@ -2928,7 +2928,7 @@
         <v>6</v>
       </c>
       <c r="E232">
-        <v>9</v>
+        <v>131</v>
       </c>
     </row>
     <row r="233" spans="1:5">
@@ -2939,7 +2939,7 @@
         <v>5</v>
       </c>
       <c r="E233">
-        <v>101</v>
+        <v>115</v>
       </c>
     </row>
     <row r="234" spans="1:5">
@@ -2950,7 +2950,7 @@
         <v>6</v>
       </c>
       <c r="E234">
-        <v>83</v>
+        <v>60</v>
       </c>
     </row>
     <row r="236" spans="1:5">
@@ -2972,7 +2972,7 @@
         <v>5</v>
       </c>
       <c r="E237">
-        <v>443</v>
+        <v>4</v>
       </c>
     </row>
     <row r="238" spans="1:5">
@@ -2983,7 +2983,7 @@
         <v>6</v>
       </c>
       <c r="E238">
-        <v>42</v>
+        <v>284</v>
       </c>
     </row>
     <row r="239" spans="1:5">
@@ -2994,7 +2994,7 @@
         <v>5</v>
       </c>
       <c r="E239">
-        <v>256</v>
+        <v>27</v>
       </c>
     </row>
     <row r="240" spans="1:5">
@@ -3005,7 +3005,7 @@
         <v>6</v>
       </c>
       <c r="E240">
-        <v>147</v>
+        <v>357</v>
       </c>
     </row>
     <row r="241" spans="1:5">
@@ -3019,7 +3019,7 @@
         <v>5</v>
       </c>
       <c r="E241">
-        <v>443</v>
+        <v>4</v>
       </c>
     </row>
     <row r="242" spans="1:5">
@@ -3030,7 +3030,7 @@
         <v>6</v>
       </c>
       <c r="E242">
-        <v>42</v>
+        <v>284</v>
       </c>
     </row>
     <row r="243" spans="1:5">
@@ -3041,7 +3041,7 @@
         <v>5</v>
       </c>
       <c r="E243">
-        <v>256</v>
+        <v>27</v>
       </c>
     </row>
     <row r="244" spans="1:5">
@@ -3052,7 +3052,7 @@
         <v>6</v>
       </c>
       <c r="E244">
-        <v>147</v>
+        <v>357</v>
       </c>
     </row>
     <row r="245" spans="1:5">
@@ -3069,7 +3069,7 @@
         <v>5</v>
       </c>
       <c r="E245">
-        <v>443</v>
+        <v>4</v>
       </c>
     </row>
     <row r="246" spans="1:5">
@@ -3080,7 +3080,7 @@
         <v>6</v>
       </c>
       <c r="E246">
-        <v>42</v>
+        <v>284</v>
       </c>
     </row>
     <row r="247" spans="1:5">
@@ -3091,7 +3091,7 @@
         <v>5</v>
       </c>
       <c r="E247">
-        <v>256</v>
+        <v>27</v>
       </c>
     </row>
     <row r="248" spans="1:5">
@@ -3102,7 +3102,7 @@
         <v>6</v>
       </c>
       <c r="E248">
-        <v>147</v>
+        <v>357</v>
       </c>
     </row>
     <row r="249" spans="1:5">
@@ -3116,7 +3116,7 @@
         <v>5</v>
       </c>
       <c r="E249">
-        <v>443</v>
+        <v>4</v>
       </c>
     </row>
     <row r="250" spans="1:5">
@@ -3127,7 +3127,7 @@
         <v>6</v>
       </c>
       <c r="E250">
-        <v>42</v>
+        <v>284</v>
       </c>
     </row>
     <row r="251" spans="1:5">
@@ -3138,7 +3138,7 @@
         <v>5</v>
       </c>
       <c r="E251">
-        <v>256</v>
+        <v>27</v>
       </c>
     </row>
     <row r="252" spans="1:5">
@@ -3149,7 +3149,7 @@
         <v>6</v>
       </c>
       <c r="E252">
-        <v>147</v>
+        <v>357</v>
       </c>
     </row>
     <row r="254" spans="1:5">
@@ -3165,7 +3165,7 @@
         <v>5</v>
       </c>
       <c r="C255">
-        <v>179</v>
+        <v>156</v>
       </c>
     </row>
     <row r="256" spans="1:5">
@@ -3173,7 +3173,7 @@
         <v>6</v>
       </c>
       <c r="C256">
-        <v>39</v>
+        <v>297</v>
       </c>
     </row>
     <row r="257" spans="1:5">
@@ -3184,7 +3184,7 @@
         <v>5</v>
       </c>
       <c r="C257">
-        <v>265</v>
+        <v>8</v>
       </c>
     </row>
     <row r="258" spans="1:5">
@@ -3192,7 +3192,7 @@
         <v>6</v>
       </c>
       <c r="C258">
-        <v>167</v>
+        <v>86</v>
       </c>
     </row>
     <row r="260" spans="1:5">
@@ -3214,7 +3214,7 @@
         <v>5</v>
       </c>
       <c r="E261">
-        <v>174</v>
+        <v>82</v>
       </c>
     </row>
     <row r="262" spans="1:5">
@@ -3225,7 +3225,7 @@
         <v>6</v>
       </c>
       <c r="E262">
-        <v>99</v>
+        <v>59</v>
       </c>
     </row>
     <row r="263" spans="1:5">
@@ -3236,7 +3236,7 @@
         <v>5</v>
       </c>
       <c r="E263">
-        <v>18</v>
+        <v>118</v>
       </c>
     </row>
     <row r="264" spans="1:5">
@@ -3247,7 +3247,7 @@
         <v>6</v>
       </c>
       <c r="E264">
-        <v>183</v>
+        <v>59</v>
       </c>
     </row>
     <row r="265" spans="1:5">
@@ -3261,7 +3261,7 @@
         <v>5</v>
       </c>
       <c r="E265">
-        <v>114</v>
+        <v>96</v>
       </c>
     </row>
     <row r="266" spans="1:5">
@@ -3272,7 +3272,7 @@
         <v>6</v>
       </c>
       <c r="E266">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="267" spans="1:5">
@@ -3283,7 +3283,7 @@
         <v>5</v>
       </c>
       <c r="E267">
-        <v>92</v>
+        <v>26</v>
       </c>
     </row>
     <row r="268" spans="1:5">
@@ -3294,7 +3294,7 @@
         <v>6</v>
       </c>
       <c r="E268">
-        <v>143</v>
+        <v>52</v>
       </c>
     </row>
     <row r="269" spans="1:5">
@@ -3311,7 +3311,7 @@
         <v>5</v>
       </c>
       <c r="E269">
-        <v>174</v>
+        <v>82</v>
       </c>
     </row>
     <row r="270" spans="1:5">
@@ -3322,7 +3322,7 @@
         <v>6</v>
       </c>
       <c r="E270">
-        <v>99</v>
+        <v>59</v>
       </c>
     </row>
     <row r="271" spans="1:5">
@@ -3333,7 +3333,7 @@
         <v>5</v>
       </c>
       <c r="E271">
-        <v>18</v>
+        <v>118</v>
       </c>
     </row>
     <row r="272" spans="1:5">
@@ -3344,7 +3344,7 @@
         <v>6</v>
       </c>
       <c r="E272">
-        <v>183</v>
+        <v>59</v>
       </c>
     </row>
     <row r="273" spans="1:5">
@@ -3358,7 +3358,7 @@
         <v>5</v>
       </c>
       <c r="E273">
-        <v>114</v>
+        <v>96</v>
       </c>
     </row>
     <row r="274" spans="1:5">
@@ -3369,7 +3369,7 @@
         <v>6</v>
       </c>
       <c r="E274">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="275" spans="1:5">
@@ -3380,7 +3380,7 @@
         <v>5</v>
       </c>
       <c r="E275">
-        <v>92</v>
+        <v>26</v>
       </c>
     </row>
     <row r="276" spans="1:5">
@@ -3391,7 +3391,7 @@
         <v>6</v>
       </c>
       <c r="E276">
-        <v>143</v>
+        <v>52</v>
       </c>
     </row>
     <row r="278" spans="1:5">
@@ -3413,7 +3413,7 @@
         <v>5</v>
       </c>
       <c r="E279">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="280" spans="1:5">
@@ -3435,7 +3435,7 @@
         <v>5</v>
       </c>
       <c r="E281">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="282" spans="1:5">
@@ -3446,7 +3446,7 @@
         <v>6</v>
       </c>
       <c r="E282">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="283" spans="1:5">
@@ -3460,7 +3460,7 @@
         <v>5</v>
       </c>
       <c r="E283">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="284" spans="1:5">
@@ -3557,7 +3557,7 @@
         <v>5</v>
       </c>
       <c r="E291">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="292" spans="1:5">
@@ -3568,7 +3568,7 @@
         <v>6</v>
       </c>
       <c r="E292">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="293" spans="1:5">
@@ -3642,7 +3642,7 @@
         <v>6</v>
       </c>
       <c r="D300">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="301" spans="1:5">
@@ -3667,7 +3667,7 @@
         <v>6</v>
       </c>
       <c r="D302">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="303" spans="1:5">
@@ -3678,7 +3678,7 @@
         <v>5</v>
       </c>
       <c r="D303">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="304" spans="1:5">
@@ -3689,7 +3689,7 @@
         <v>6</v>
       </c>
       <c r="D304">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>